<commit_message>
Update address for Srinivasa Trust and delete 1 trust that has been closed .
</commit_message>
<xml_diff>
--- a/resources/AddressList.xlsx
+++ b/resources/AddressList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Clients\probono\code\gsb-scholarship.github.io\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E6D870-D518-471C-8474-243A622BEB95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94406EDE-BBC5-445A-9FB6-9499C5E494F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3D82F0E1-B268-4301-A975-E905FDB967A5}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="66">
   <si>
     <t>SI</t>
   </si>
@@ -60,12 +60,6 @@
     <t>Welfare Fund, Regd. Office, Sukratindra Sabha Sadan, SLV Temple, Udupi - 576101</t>
   </si>
   <si>
-    <t>Sri Srinivas Kalyan Mantap Trust</t>
-  </si>
-  <si>
-    <t>139/ 8th Main, Malleshwaram, Bengaluru - 560003</t>
-  </si>
-  <si>
     <t>Sri Venkatesh Seva Dal</t>
   </si>
   <si>
@@ -111,12 +105,6 @@
     <t>Sri Ram Nayak, Mahamaya Temple, Bantwal - 574211, Karnataka</t>
   </si>
   <si>
-    <t>Arkul Vittal Shenoy Charitable Trust</t>
-  </si>
-  <si>
-    <t>140/8th Main Road, 15th Cross, Malleshwaram, Bengaluru - 560003\</t>
-  </si>
-  <si>
     <t>Sri Laxmi Venkataramana Seva Trust</t>
   </si>
   <si>
@@ -223,6 +211,20 @@
   </si>
   <si>
     <t>President, GSB Sabha, Kurla Chembur, Ghatkopar, Near Railway Station, Balaji Mandir, Kurla, Mumbai - 400070</t>
+  </si>
+  <si>
+    <t>M/s.Srinivasa Kalyana Mantap Trust</t>
+  </si>
+  <si>
+    <t>Off: No 9, Sri Ganesh Building 
+4th cross Link Road,  
+P O Box no 386 , Malleswaram 8th cross post office,  Malleshwaram, Bangalore- 560003</t>
+  </si>
+  <si>
+    <t>skmtrust1967@gmail.com</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -981,8 +983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EC88F57-C99F-428D-96C3-078A1595D8E9}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection sqref="A1:G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1013,13 +1015,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>4</v>
@@ -1039,7 +1041,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
@@ -1055,10 +1057,10 @@
         <v>8</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
@@ -1077,7 +1079,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
@@ -1085,22 +1087,26 @@
       <c r="H4" s="6"/>
       <c r="I4" s="7"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>11</v>
+        <v>62</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>12</v>
+        <v>63</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="E5" s="6"/>
+        <v>65</v>
+      </c>
+      <c r="E5" s="6">
+        <v>9916611828</v>
+      </c>
       <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
+      <c r="G5" s="12" t="s">
+        <v>64</v>
+      </c>
       <c r="H5" s="6"/>
       <c r="I5" s="7"/>
     </row>
@@ -1109,13 +1115,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
@@ -1128,13 +1134,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
@@ -1147,13 +1153,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -1166,13 +1172,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -1185,13 +1191,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
@@ -1204,22 +1210,22 @@
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="7"/>
@@ -1229,13 +1235,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>27</v>
-      </c>
       <c r="D12" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
@@ -1243,18 +1249,18 @@
       <c r="H12" s="6"/>
       <c r="I12" s="7"/>
     </row>
-    <row r="13" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
@@ -1267,13 +1273,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
@@ -1281,58 +1287,58 @@
       <c r="H14" s="6"/>
       <c r="I14" s="7"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>33</v>
-      </c>
       <c r="D15" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
+      <c r="F15" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E16" s="6"/>
-      <c r="F16" s="12" t="s">
-        <v>41</v>
-      </c>
+      <c r="F16" s="12"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
       <c r="I16" s="7"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
@@ -1345,13 +1351,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
@@ -1359,18 +1365,18 @@
       <c r="H18" s="6"/>
       <c r="I18" s="7"/>
     </row>
-    <row r="19" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
@@ -1378,18 +1384,18 @@
       <c r="H19" s="6"/>
       <c r="I19" s="7"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
@@ -1397,18 +1403,18 @@
       <c r="H20" s="6"/>
       <c r="I20" s="7"/>
     </row>
-    <row r="21" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
@@ -1421,13 +1427,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
@@ -1435,18 +1441,18 @@
       <c r="H22" s="6"/>
       <c r="I22" s="7"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
@@ -1459,13 +1465,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
@@ -1478,13 +1484,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
@@ -1497,13 +1503,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
@@ -1511,19 +1517,11 @@
       <c r="H26" s="6"/>
       <c r="I26" s="7"/>
     </row>
-    <row r="27" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="5">
-        <v>26</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>63</v>
-      </c>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="5"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
@@ -1531,9 +1529,7 @@
       <c r="I27" s="7"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="5">
-        <v>27</v>
-      </c>
+      <c r="A28" s="5"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
@@ -1544,9 +1540,7 @@
       <c r="I28" s="7"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="8">
-        <v>28</v>
-      </c>
+      <c r="A29" s="8"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
@@ -1560,16 +1554,18 @@
   <hyperlinks>
     <hyperlink ref="G11" r:id="rId1" xr:uid="{FD797D9F-929B-4DBB-9FE9-C9B1B32DA5C5}"/>
     <hyperlink ref="F11" r:id="rId2" xr:uid="{B9E7ECA6-5C1E-45AD-9316-FDB54885BC60}"/>
-    <hyperlink ref="F16" r:id="rId3" xr:uid="{FDE5DA47-A083-45C6-89CD-FD8DAB027F3C}"/>
+    <hyperlink ref="F16" r:id="rId3" display="https://vishwakonkani.org/scholarships/" xr:uid="{FDE5DA47-A083-45C6-89CD-FD8DAB027F3C}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{CEF26D58-6D08-4A94-858A-F73BDCF23D7C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>
-  <webPublishItems count="2">
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId5"/>
+  <webPublishItems count="3">
+    <webPublishItem id="15881" divId="AddressList_15881" sourceType="range" sourceRef="A1:G26" destinationFile="D:\Work\Clients\probono\code\gsb-scholarship.github.io\resources\AddressList_20210825.htm" title="GSB Scholarship List"/>
     <webPublishItem id="6097" divId="AddressList_6097" sourceType="range" sourceRef="A1:G27" destinationFile="D:\Work\Clients\probono\code\gsb-scholarship.github.io\resources\AddressList.htm" title="GSB Scholarship List"/>
     <webPublishItem id="27094" divId="AddressList_27094" sourceType="range" sourceRef="A1:I27" destinationFile="D:\Work\Clients\probono\code\gsb-scholarship.github.io\resources\AddressList.htm" title="List of Charitable Institutes and other details"/>
   </webPublishItems>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
remove phone number of Srinivasa Trust on request. Prefered contact mail
</commit_message>
<xml_diff>
--- a/resources/AddressList.xlsx
+++ b/resources/AddressList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Clients\probono\code\gsb-scholarship.github.io\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94406EDE-BBC5-445A-9FB6-9499C5E494F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC3E5AC-F9A2-4BE8-BE88-77FFFA80620B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3D82F0E1-B268-4301-A975-E905FDB967A5}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="66">
   <si>
     <t>SI</t>
   </si>
@@ -438,6 +438,25 @@
   <dxfs count="14">
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -466,25 +485,6 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -674,11 +674,11 @@
     <tableColumn id="2" xr3:uid="{003443F8-D4E2-4413-B7AF-E8B73EFCA521}" name="Institute" dataDxfId="7"/>
     <tableColumn id="3" xr3:uid="{5F77DE74-7B72-41EE-A698-CE988F64C8A0}" name="Address" dataDxfId="6"/>
     <tableColumn id="4" xr3:uid="{179A95E7-C783-472E-A28A-E62B5A1E94C1}" name="Verified" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{3ED6DEAC-58B8-4FB3-87DF-60FA79E1D02A}" name="Contact Number" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{359B94DA-6D44-4983-8D8C-F8375F65B0CB}" name="Website" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{C16A54C2-A090-4E60-80BC-A11AECC895D4}" name="Email" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{8BC79951-4557-4FE5-8DAD-331E5E923CF7}" name="Classes" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{B18544C0-0EB4-4484-B2C3-68A25BDFDD15}" name="Type of Scholarship" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{3ED6DEAC-58B8-4FB3-87DF-60FA79E1D02A}" name="Contact Number" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{359B94DA-6D44-4983-8D8C-F8375F65B0CB}" name="Website" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{C16A54C2-A090-4E60-80BC-A11AECC895D4}" name="Email" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{8BC79951-4557-4FE5-8DAD-331E5E923CF7}" name="Classes" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{B18544C0-0EB4-4484-B2C3-68A25BDFDD15}" name="Type of Scholarship" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -981,10 +981,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EC88F57-C99F-428D-96C3-078A1595D8E9}">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection sqref="A1:G26"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -998,10 +998,11 @@
     <col min="7" max="7" width="27.109375" style="4" customWidth="1"/>
     <col min="8" max="8" width="14.88671875" style="4" customWidth="1"/>
     <col min="9" max="9" width="25.33203125" style="4" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="4"/>
+    <col min="10" max="10" width="20.88671875" style="4" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1029,8 +1030,11 @@
       <c r="I1" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J1" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1048,8 +1052,9 @@
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="7"/>
-    </row>
-    <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J2" s="6"/>
+    </row>
+    <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1067,8 +1072,9 @@
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="7"/>
-    </row>
-    <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J3" s="6"/>
+    </row>
+    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1086,8 +1092,9 @@
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="7"/>
-    </row>
-    <row r="5" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="J4" s="6"/>
+    </row>
+    <row r="5" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1100,17 +1107,18 @@
       <c r="D5" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="E5" s="6">
-        <v>9916611828</v>
-      </c>
+      <c r="E5" s="6"/>
       <c r="F5" s="6"/>
       <c r="G5" s="12" t="s">
         <v>64</v>
       </c>
       <c r="H5" s="6"/>
       <c r="I5" s="7"/>
-    </row>
-    <row r="6" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J5" s="6">
+        <v>9916611828</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1128,8 +1136,9 @@
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="7"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J6" s="6"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -1147,8 +1156,9 @@
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
       <c r="I7" s="7"/>
-    </row>
-    <row r="8" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -1166,8 +1176,9 @@
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="7"/>
-    </row>
-    <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -1185,8 +1196,9 @@
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="7"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J9" s="6"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -1204,8 +1216,9 @@
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="7"/>
-    </row>
-    <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J10" s="6"/>
+    </row>
+    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -1229,8 +1242,11 @@
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="7"/>
-    </row>
-    <row r="12" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J11" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -1248,8 +1264,9 @@
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
       <c r="I12" s="7"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J12" s="6"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -1267,8 +1284,9 @@
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
       <c r="I13" s="7"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J13" s="6"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1286,8 +1304,9 @@
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
       <c r="I14" s="7"/>
-    </row>
-    <row r="15" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="J14" s="6"/>
+    </row>
+    <row r="15" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -1307,8 +1326,9 @@
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
       <c r="I15" s="7"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J15" s="6"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -1326,8 +1346,9 @@
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
       <c r="I16" s="7"/>
-    </row>
-    <row r="17" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J16" s="6"/>
+    </row>
+    <row r="17" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -1345,8 +1366,9 @@
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="7"/>
-    </row>
-    <row r="18" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J17" s="6"/>
+    </row>
+    <row r="18" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -1364,8 +1386,9 @@
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
       <c r="I18" s="7"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J18" s="6"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -1383,8 +1406,9 @@
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
       <c r="I19" s="7"/>
-    </row>
-    <row r="20" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J19" s="6"/>
+    </row>
+    <row r="20" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -1402,8 +1426,9 @@
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
       <c r="I20" s="7"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J20" s="6"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -1421,8 +1446,9 @@
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
       <c r="I21" s="7"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J21" s="6"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -1440,8 +1466,9 @@
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
       <c r="I22" s="7"/>
-    </row>
-    <row r="23" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J22" s="6"/>
+    </row>
+    <row r="23" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -1459,8 +1486,9 @@
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
       <c r="I23" s="7"/>
-    </row>
-    <row r="24" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J23" s="6"/>
+    </row>
+    <row r="24" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -1478,8 +1506,9 @@
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
       <c r="I24" s="7"/>
-    </row>
-    <row r="25" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J24" s="6"/>
+    </row>
+    <row r="25" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -1497,8 +1526,9 @@
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
       <c r="I25" s="7"/>
-    </row>
-    <row r="26" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J25" s="6"/>
+    </row>
+    <row r="26" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -1516,8 +1546,9 @@
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
       <c r="I26" s="7"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J26" s="6"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -1527,8 +1558,9 @@
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
       <c r="I27" s="7"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J27" s="6"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
@@ -1538,8 +1570,9 @@
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
       <c r="I28" s="7"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J28" s="6"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="8"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -1549,6 +1582,7 @@
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
       <c r="I29" s="10"/>
+      <c r="J29" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
update information in excel
</commit_message>
<xml_diff>
--- a/resources/AddressList.xlsx
+++ b/resources/AddressList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Clients\probono\code\gsb-scholarship.github.io\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC3E5AC-F9A2-4BE8-BE88-77FFFA80620B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5BB8367-170C-42C1-B706-1D3ABC81E684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3D82F0E1-B268-4301-A975-E905FDB967A5}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="74">
   <si>
     <t>SI</t>
   </si>
@@ -225,6 +225,31 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>10, PUC, degree and all 3, 4 and 5 year professional courses</t>
+  </si>
+  <si>
+    <t>Scholarship based on financial situation</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Non Bangalore</t>
+  </si>
+  <si>
+    <t>Process</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Varies based on number of applications received that year</t>
+  </si>
+  <si>
+    <t>Candidates to Share their name, address , and class studying to postal address or a request letter for application form , by post. 
+We then send the scholarship application by post which needs to be filled up and all attachments to be sent along with the application by post/ courier.</t>
   </si>
 </sst>
 </file>
@@ -394,7 +419,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -430,30 +455,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="16">
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -667,18 +685,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{61128AE1-3139-44D4-AA7F-DB7CDFCF178B}" name="Table1" displayName="Table1" ref="A1:I29" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" totalsRowBorderDxfId="9">
-  <autoFilter ref="A1:I29" xr:uid="{61128AE1-3139-44D4-AA7F-DB7CDFCF178B}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{0A294F43-8CC1-410B-BFA0-18E7555A13C0}" name="SI" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{003443F8-D4E2-4413-B7AF-E8B73EFCA521}" name="Institute" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{5F77DE74-7B72-41EE-A698-CE988F64C8A0}" name="Address" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{179A95E7-C783-472E-A28A-E62B5A1E94C1}" name="Verified" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{3ED6DEAC-58B8-4FB3-87DF-60FA79E1D02A}" name="Contact Number" dataDxfId="0"/>
-    <tableColumn id="8" xr3:uid="{359B94DA-6D44-4983-8D8C-F8375F65B0CB}" name="Website" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{C16A54C2-A090-4E60-80BC-A11AECC895D4}" name="Email" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{8BC79951-4557-4FE5-8DAD-331E5E923CF7}" name="Classes" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{B18544C0-0EB4-4484-B2C3-68A25BDFDD15}" name="Type of Scholarship" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{61128AE1-3139-44D4-AA7F-DB7CDFCF178B}" name="Table1" displayName="Table1" ref="A1:K29" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+  <autoFilter ref="A1:K29" xr:uid="{61128AE1-3139-44D4-AA7F-DB7CDFCF178B}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{0A294F43-8CC1-410B-BFA0-18E7555A13C0}" name="SI" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{003443F8-D4E2-4413-B7AF-E8B73EFCA521}" name="Institute" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{5F77DE74-7B72-41EE-A698-CE988F64C8A0}" name="Address" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{179A95E7-C783-472E-A28A-E62B5A1E94C1}" name="Verified" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{359B94DA-6D44-4983-8D8C-F8375F65B0CB}" name="Website" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{C16A54C2-A090-4E60-80BC-A11AECC895D4}" name="Email" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{8BC79951-4557-4FE5-8DAD-331E5E923CF7}" name="Classes" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{B18544C0-0EB4-4484-B2C3-68A25BDFDD15}" name="Type of Scholarship" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{2F77FD5C-E446-40BF-9A08-CCEEB9121D3B}" name="Region" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{28785629-5BB6-423A-B32A-DA2C67ED8CE7}" name="Process" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{6CC73244-1B7F-452C-B244-1B5C41063AD1}" name="Amount" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -981,10 +1001,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EC88F57-C99F-428D-96C3-078A1595D8E9}">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -993,16 +1013,15 @@
     <col min="2" max="2" width="34.109375" style="4" customWidth="1"/>
     <col min="3" max="3" width="47.5546875" style="4" customWidth="1"/>
     <col min="4" max="4" width="9.44140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="20.88671875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="36.109375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="27.109375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="14.88671875" style="4" customWidth="1"/>
-    <col min="9" max="9" width="25.33203125" style="4" customWidth="1"/>
-    <col min="10" max="10" width="20.88671875" style="4" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="4"/>
+    <col min="5" max="5" width="36.109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="27.109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="14.88671875" style="4" customWidth="1"/>
+    <col min="8" max="11" width="25.33203125" style="4" customWidth="1"/>
+    <col min="12" max="12" width="20.88671875" style="4" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1016,25 +1035,31 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1050,11 +1075,13 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
+      <c r="H2" s="7"/>
       <c r="I2" s="7"/>
-      <c r="J2" s="6"/>
-    </row>
-    <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="6"/>
+    </row>
+    <row r="3" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1070,11 +1097,13 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
+      <c r="H3" s="7"/>
       <c r="I3" s="7"/>
-      <c r="J3" s="6"/>
-    </row>
-    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="6"/>
+    </row>
+    <row r="4" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1090,11 +1119,13 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
+      <c r="H4" s="7"/>
       <c r="I4" s="7"/>
-      <c r="J4" s="6"/>
-    </row>
-    <row r="5" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="6"/>
+    </row>
+    <row r="5" spans="1:12" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1108,17 +1139,29 @@
         <v>65</v>
       </c>
       <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="12" t="s">
+      <c r="F5" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="6">
+      <c r="G5" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="L5" s="6">
         <v>9916611828</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1134,11 +1177,13 @@
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
+      <c r="H6" s="7"/>
       <c r="I6" s="7"/>
-      <c r="J6" s="6"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="6"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -1154,11 +1199,13 @@
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
+      <c r="H7" s="7"/>
       <c r="I7" s="7"/>
-      <c r="J7" s="6"/>
-    </row>
-    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="6"/>
+    </row>
+    <row r="8" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -1174,11 +1221,13 @@
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
+      <c r="H8" s="7"/>
       <c r="I8" s="7"/>
-      <c r="J8" s="6"/>
-    </row>
-    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="6"/>
+    </row>
+    <row r="9" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -1194,11 +1243,13 @@
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
+      <c r="H9" s="7"/>
       <c r="I9" s="7"/>
-      <c r="J9" s="6"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="6"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -1214,11 +1265,13 @@
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
+      <c r="H10" s="7"/>
       <c r="I10" s="7"/>
-      <c r="J10" s="6"/>
-    </row>
-    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="6"/>
+    </row>
+    <row r="11" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -1231,22 +1284,22 @@
       <c r="D11" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="6"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="H11" s="6"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -1262,11 +1315,13 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
+      <c r="H12" s="7"/>
       <c r="I12" s="7"/>
-      <c r="J12" s="6"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="6"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -1282,11 +1337,13 @@
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
+      <c r="H13" s="7"/>
       <c r="I13" s="7"/>
-      <c r="J13" s="6"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="6"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1302,11 +1359,13 @@
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
+      <c r="H14" s="7"/>
       <c r="I14" s="7"/>
-      <c r="J14" s="6"/>
-    </row>
-    <row r="15" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="6"/>
+    </row>
+    <row r="15" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -1319,16 +1378,18 @@
       <c r="D15" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6" t="s">
+      <c r="E15" s="6" t="s">
         <v>37</v>
       </c>
+      <c r="F15" s="6"/>
       <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
+      <c r="H15" s="7"/>
       <c r="I15" s="7"/>
-      <c r="J15" s="6"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="6"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -1341,14 +1402,16 @@
       <c r="D16" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="6"/>
       <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
+      <c r="H16" s="7"/>
       <c r="I16" s="7"/>
-      <c r="J16" s="6"/>
-    </row>
-    <row r="17" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="6"/>
+    </row>
+    <row r="17" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -1364,11 +1427,13 @@
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
+      <c r="H17" s="7"/>
       <c r="I17" s="7"/>
-      <c r="J17" s="6"/>
-    </row>
-    <row r="18" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="6"/>
+    </row>
+    <row r="18" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -1384,11 +1449,13 @@
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
+      <c r="H18" s="7"/>
       <c r="I18" s="7"/>
-      <c r="J18" s="6"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="6"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -1404,11 +1471,13 @@
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
+      <c r="H19" s="7"/>
       <c r="I19" s="7"/>
-      <c r="J19" s="6"/>
-    </row>
-    <row r="20" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="6"/>
+    </row>
+    <row r="20" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -1424,11 +1493,13 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
+      <c r="H20" s="7"/>
       <c r="I20" s="7"/>
-      <c r="J20" s="6"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="6"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -1444,11 +1515,13 @@
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
+      <c r="H21" s="7"/>
       <c r="I21" s="7"/>
-      <c r="J21" s="6"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="6"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -1464,11 +1537,13 @@
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
+      <c r="H22" s="7"/>
       <c r="I22" s="7"/>
-      <c r="J22" s="6"/>
-    </row>
-    <row r="23" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="6"/>
+    </row>
+    <row r="23" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -1484,11 +1559,13 @@
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
+      <c r="H23" s="7"/>
       <c r="I23" s="7"/>
-      <c r="J23" s="6"/>
-    </row>
-    <row r="24" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="6"/>
+    </row>
+    <row r="24" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -1504,11 +1581,13 @@
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
+      <c r="H24" s="7"/>
       <c r="I24" s="7"/>
-      <c r="J24" s="6"/>
-    </row>
-    <row r="25" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="6"/>
+    </row>
+    <row r="25" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -1524,11 +1603,13 @@
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
+      <c r="H25" s="7"/>
       <c r="I25" s="7"/>
-      <c r="J25" s="6"/>
-    </row>
-    <row r="26" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="6"/>
+    </row>
+    <row r="26" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -1544,11 +1625,13 @@
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
+      <c r="H26" s="7"/>
       <c r="I26" s="7"/>
-      <c r="J26" s="6"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="6"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -1556,11 +1639,13 @@
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
+      <c r="H27" s="7"/>
       <c r="I27" s="7"/>
-      <c r="J27" s="6"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="6"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
@@ -1568,11 +1653,13 @@
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
+      <c r="H28" s="7"/>
       <c r="I28" s="7"/>
-      <c r="J28" s="6"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="6"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="8"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -1580,23 +1667,25 @@
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
+      <c r="H29" s="10"/>
       <c r="I29" s="10"/>
-      <c r="J29" s="9"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G11" r:id="rId1" xr:uid="{FD797D9F-929B-4DBB-9FE9-C9B1B32DA5C5}"/>
-    <hyperlink ref="F11" r:id="rId2" xr:uid="{B9E7ECA6-5C1E-45AD-9316-FDB54885BC60}"/>
-    <hyperlink ref="F16" r:id="rId3" display="https://vishwakonkani.org/scholarships/" xr:uid="{FDE5DA47-A083-45C6-89CD-FD8DAB027F3C}"/>
-    <hyperlink ref="G5" r:id="rId4" xr:uid="{CEF26D58-6D08-4A94-858A-F73BDCF23D7C}"/>
+    <hyperlink ref="F11" r:id="rId1" xr:uid="{FD797D9F-929B-4DBB-9FE9-C9B1B32DA5C5}"/>
+    <hyperlink ref="E11" r:id="rId2" xr:uid="{B9E7ECA6-5C1E-45AD-9316-FDB54885BC60}"/>
+    <hyperlink ref="E16" r:id="rId3" display="https://vishwakonkani.org/scholarships/" xr:uid="{FDE5DA47-A083-45C6-89CD-FD8DAB027F3C}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{CEF26D58-6D08-4A94-858A-F73BDCF23D7C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId5"/>
   <webPublishItems count="3">
-    <webPublishItem id="15881" divId="AddressList_15881" sourceType="range" sourceRef="A1:G26" destinationFile="D:\Work\Clients\probono\code\gsb-scholarship.github.io\resources\AddressList_20210825.htm" title="GSB Scholarship List"/>
-    <webPublishItem id="6097" divId="AddressList_6097" sourceType="range" sourceRef="A1:G27" destinationFile="D:\Work\Clients\probono\code\gsb-scholarship.github.io\resources\AddressList.htm" title="GSB Scholarship List"/>
-    <webPublishItem id="27094" divId="AddressList_27094" sourceType="range" sourceRef="A1:I27" destinationFile="D:\Work\Clients\probono\code\gsb-scholarship.github.io\resources\AddressList.htm" title="List of Charitable Institutes and other details"/>
+    <webPublishItem id="15881" divId="AddressList_15881" sourceType="range" sourceRef="A1:F26" destinationFile="D:\Work\Clients\probono\code\gsb-scholarship.github.io\resources\AddressList_20210825.htm" title="GSB Scholarship List"/>
+    <webPublishItem id="6097" divId="AddressList_6097" sourceType="range" sourceRef="A1:F27" destinationFile="D:\Work\Clients\probono\code\gsb-scholarship.github.io\resources\AddressList.htm" title="GSB Scholarship List"/>
+    <webPublishItem id="27094" divId="AddressList_27094" sourceType="range" sourceRef="A1:H27" destinationFile="D:\Work\Clients\probono\code\gsb-scholarship.github.io\resources\AddressList.htm" title="List of Charitable Institutes and other details"/>
   </webPublishItems>
   <tableParts count="1">
     <tablePart r:id="rId6"/>

</xml_diff>